<commit_message>
edit import list topic
</commit_message>
<xml_diff>
--- a/public/assets/KTLN - template import ds đề tài.xlsx
+++ b/public/assets/KTLN - template import ds đề tài.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A! Template KLTN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB7D12D-2F0E-4004-9D81-B6D327D6FFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179051C8-8BD7-4EE3-8CBF-FD1EC5C333FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="134">
   <si>
     <t>STT</t>
   </si>
@@ -336,13 +336,146 @@
   </si>
   <si>
     <t>Human resource management app</t>
+  </si>
+  <si>
+    <t>MSSV</t>
+  </si>
+  <si>
+    <t>SĐT</t>
+  </si>
+  <si>
+    <t>Nguyễn Hoàng Linh
+Lê Thành Lộc</t>
+  </si>
+  <si>
+    <t>0378060972
+0356728919</t>
+  </si>
+  <si>
+    <t>21522289
+21521087</t>
+  </si>
+  <si>
+    <t>21525432_x000D_
+21526789</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị C_x000D_
+Lê Văn D</t>
+  </si>
+  <si>
+    <t>21529012_x000D_
+21527891</t>
+  </si>
+  <si>
+    <t>Hoàng Thị E_x000D_
+Đỗ Minh F</t>
+  </si>
+  <si>
+    <t>21531234_x000D_
+21530123</t>
+  </si>
+  <si>
+    <t>Phan Hữu G_x000D_
+Trịnh Anh H</t>
+  </si>
+  <si>
+    <t>21535467_x000D_
+21534512</t>
+  </si>
+  <si>
+    <t>Vũ Hải K_x000D_
+Ngô Thanh L</t>
+  </si>
+  <si>
+    <t>21539876_x000D_
+21538765</t>
+  </si>
+  <si>
+    <t>Đinh Việt M_x000D_
+Bùi Thị N</t>
+  </si>
+  <si>
+    <t>21540987_x000D_
+21549876</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh P_x000D_
+Trần Thị Q</t>
+  </si>
+  <si>
+    <t>21542034_x000D_
+21543012</t>
+  </si>
+  <si>
+    <t>Phạm Quốc R_x000D_
+Đỗ Ngọc S</t>
+  </si>
+  <si>
+    <t>21546789_x000D_
+21545678</t>
+  </si>
+  <si>
+    <t>Lê Hoàng T_x000D_
+Nguyễn Văn U</t>
+  </si>
+  <si>
+    <t>21547890_x000D_
+21548901</t>
+  </si>
+  <si>
+    <t>Đặng Quốc V_x000D_
+Trịnh Thị W</t>
+  </si>
+  <si>
+    <t>21551234_x000D_
+21552345</t>
+  </si>
+  <si>
+    <t>Vũ Văn X_x000D_
+Lê Minh Y</t>
+  </si>
+  <si>
+    <t>21556789_x000D_
+21555678</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Z_x000D_
+Phạm Thị AA</t>
+  </si>
+  <si>
+    <t>21559876_x000D_
+21558965</t>
+  </si>
+  <si>
+    <t>Đỗ Văn AB_x000D_
+Bùi Thị AC</t>
+  </si>
+  <si>
+    <t>21561234_x000D_
+21562345</t>
+  </si>
+  <si>
+    <t>Trần Hoài AD_x000D_
+Nguyễn Thị AE</t>
+  </si>
+  <si>
+    <t>21567890_x000D_
+21568901</t>
+  </si>
+  <si>
+    <t>Phạm Quốc AF_x000D_
+Đinh Hải AG</t>
+  </si>
+  <si>
+    <t>Họ và tên</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -363,6 +496,19 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -385,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -407,6 +553,18 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -749,984 +907,1240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="4"/>
-    <col min="2" max="3" width="30.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="93.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="4"/>
+    <col min="2" max="2" width="12.21875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="39.21875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="93.44140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="4"/>
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="4"/>
+      <c r="F1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="H12" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="H14" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>13</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>14</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="H16" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>15</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="G17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="H17" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>16</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="H18" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>17</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="H19" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>18</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="G20" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="H20" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>19</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="H21" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>20</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="F22" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="H22" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>21</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="H23" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>22</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="10"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="F24" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="G24" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="H24" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>23</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="H25" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>24</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="G26" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="H26" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>25</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>26</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="F28" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="G28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="H28" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>27</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="H29" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>28</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="10"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="F30" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="G30" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="H30" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>29</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="G31" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="H31" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>30</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="F32" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="G32" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="H32" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>31</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="10"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="F33" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="G33" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="H33" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>32</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="H34" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>33</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="G35" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="H35" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>34</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="F36" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="G36" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="H36" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>35</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="F37" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="G37" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="H37" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>36</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="F38" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="G38" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="H38" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>37</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="G39" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="H39" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>38</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="10"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="F40" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="G40" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="H40" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>39</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="H41" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>40</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="F42" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="G42" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="H42" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>41</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="G43" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="H43" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>42</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="G44" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="H44" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="G45" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="H45" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>44</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="10"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="F46" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="G46" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="H46" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>45</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="F47" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="G47" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="H47" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>46</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="F48" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="G48" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="H48" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>47</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="F49" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="G49" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="H49" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>48</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="F50" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="G50" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="H50" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>49</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="F51" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="G51" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="H51" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>50</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="10"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="F52" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="G52" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E52" s="7" t="s">
+      <c r="H52" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>51</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="F53" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="G53" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="H53" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>52</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="F54" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="G54" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="H54" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>53</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="F55" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="G55" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="H55" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>54</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="F56" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="G56" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="H56" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>55</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="F57" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="G57" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="H57" s="7" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
-    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.13888888888889001" right="0.13888888888889001" top="0.69444444444443998" bottom="0.69444444444443998" header="0" footer="0"/>

</xml_diff>